<commit_message>
Apply constraints from 2022
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_IND_Mitigations.xlsx
+++ b/SuppXLS/Scen_B_IND_Mitigations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39AB1C3-35B3-40AD-85F2-7301C7BFC3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856EEE94-0A29-4B6B-B434-4D3ED4E9B19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -742,9 +742,6 @@
     <t>Biofuels max substitutions</t>
   </si>
   <si>
-    <t>UC_RHSRTS~2018</t>
-  </si>
-  <si>
     <t>~UC_T: UC_FLO</t>
   </si>
   <si>
@@ -833,6 +830,9 @@
   </si>
   <si>
     <t>*2021</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS~2022</t>
   </si>
 </sst>
 </file>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B16" s="58"/>
       <c r="C16" s="58"/>
@@ -2502,10 +2502,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" s="57"/>
       <c r="D19" s="57"/>
@@ -2534,10 +2534,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C20" s="57"/>
       <c r="D20" s="57"/>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C21" s="52"/>
       <c r="D21" s="52"/>
@@ -2626,10 +2626,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
@@ -2659,7 +2659,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" s="57"/>
       <c r="D24" s="57"/>
@@ -2689,7 +2689,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49"/>
       <c r="B25" s="57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" s="57"/>
       <c r="D25" s="57"/>
@@ -2718,10 +2718,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C26" s="57"/>
       <c r="D26" s="57"/>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" s="53">
         <v>1</v>
@@ -2838,10 +2838,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" s="59" t="s">
         <v>154</v>
-      </c>
-      <c r="B30" s="59" t="s">
-        <v>155</v>
       </c>
       <c r="C30" s="57"/>
       <c r="D30" s="57"/>
@@ -2870,10 +2870,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="57" t="s">
         <v>156</v>
-      </c>
-      <c r="B31" s="57" t="s">
-        <v>157</v>
       </c>
       <c r="C31" s="57"/>
       <c r="D31" s="57"/>
@@ -2903,7 +2903,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
       <c r="B32" s="56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C32" s="55"/>
       <c r="D32" s="55"/>
@@ -5599,8 +5599,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:AG147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T72" sqref="T72"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5674,7 +5674,7 @@
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="AA4" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
@@ -5748,13 +5748,13 @@
         <v>64</v>
       </c>
       <c r="Z5" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA5" s="10" t="s">
         <v>60</v>
       </c>
       <c r="AB5" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AC5" s="10">
         <v>2022</v>
@@ -5766,7 +5766,7 @@
         <v>2050</v>
       </c>
       <c r="AF5" s="10" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="AG5" s="10" t="s">
         <v>127</v>
@@ -5790,7 +5790,7 @@
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
@@ -5872,10 +5872,10 @@
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="Y7" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z7" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA7" s="22" t="s">
         <v>131</v>
@@ -5946,10 +5946,10 @@
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="Y8" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z8" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA8" s="22" t="s">
         <v>131</v>
@@ -6036,7 +6036,7 @@
         <v>IND*</v>
       </c>
       <c r="Z9" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA9" s="22" t="str">
         <f>$AA$7</f>
@@ -6111,10 +6111,10 @@
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="Y10" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z10" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA10" s="22" t="str">
         <f>$AA$7</f>
@@ -6192,7 +6192,7 @@
         <v>IND*</v>
       </c>
       <c r="Z11" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA11" s="22" t="str">
         <f>$AA$7</f>
@@ -6283,10 +6283,10 @@
         <v>I-DMD-NEM-E0</v>
       </c>
       <c r="Y12" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z12" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA12" s="22" t="str">
         <f>$AA$7</f>
@@ -6525,10 +6525,10 @@
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="Y16" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z16" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA16" s="34" t="str">
         <f>$AA$20</f>
@@ -6593,10 +6593,10 @@
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="Y17" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z17" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA17" s="34" t="str">
         <f>$AA$20</f>
@@ -6682,7 +6682,7 @@
         <v>IND*</v>
       </c>
       <c r="Z18" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA18" s="34" t="str">
         <f>$AA$20</f>
@@ -6753,10 +6753,10 @@
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="Y19" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z19" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA19" s="34" t="str">
         <f>$AA$20</f>
@@ -6833,7 +6833,7 @@
         <v>IND*</v>
       </c>
       <c r="Z20" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA20" s="22" t="s">
         <v>131</v>
@@ -6906,10 +6906,10 @@
         <v>I-DMD-FAB-E0</v>
       </c>
       <c r="Y21" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z21" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA21" s="22" t="s">
         <v>131</v>
@@ -7335,10 +7335,10 @@
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="Y29" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z29" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA29" s="34" t="str">
         <f>$AA$20</f>
@@ -7409,10 +7409,10 @@
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="Y30" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z30" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA30" s="34" t="str">
         <f>$AA$20</f>
@@ -7498,7 +7498,7 @@
         <v>IND*</v>
       </c>
       <c r="Z31" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA31" s="34" t="str">
         <f>$AA$20</f>
@@ -7578,10 +7578,10 @@
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="Y32" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z32" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA32" s="34" t="str">
         <f>$AA$20</f>
@@ -7652,7 +7652,7 @@
         <v>IND*</v>
       </c>
       <c r="Z33" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA33" s="22" t="s">
         <v>131</v>
@@ -7688,7 +7688,7 @@
         <v>76</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>109</v>
@@ -7740,10 +7740,10 @@
         <v>I-DMD-TAP-E0</v>
       </c>
       <c r="Y34" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z34" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA34" s="22" t="s">
         <v>131</v>
@@ -7773,7 +7773,7 @@
         <v>76</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>110</v>
@@ -7832,7 +7832,7 @@
         <v>76</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>80</v>
@@ -7892,10 +7892,10 @@
         <v>76</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>98</v>
@@ -7980,10 +7980,10 @@
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="Y38" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z38" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA38" s="34" t="str">
         <f>$AA$20</f>
@@ -8054,10 +8054,10 @@
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="Y39" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z39" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA39" s="34" t="str">
         <f>$AA$20</f>
@@ -8143,7 +8143,7 @@
         <v>IND*</v>
       </c>
       <c r="Z40" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA40" s="34" t="str">
         <f>$AA$20</f>
@@ -8223,10 +8223,10 @@
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="Y41" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z41" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA41" s="34" t="str">
         <f>$AA$20</f>
@@ -8297,7 +8297,7 @@
         <v>IND*</v>
       </c>
       <c r="Z42" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA42" s="22" t="s">
         <v>131</v>
@@ -8367,10 +8367,10 @@
         <v>I-DMD-WAP-E0</v>
       </c>
       <c r="Y43" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z43" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA43" s="22" t="s">
         <v>131</v>
@@ -8666,10 +8666,10 @@
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="Y48" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z48" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA48" s="34" t="str">
         <f>$AA$20</f>
@@ -8740,10 +8740,10 @@
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="Y49" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z49" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA49" s="34" t="str">
         <f>$AA$20</f>
@@ -8823,7 +8823,7 @@
         <v>IND*</v>
       </c>
       <c r="Z50" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA50" s="34" t="str">
         <f>$AA$20</f>
@@ -8903,10 +8903,10 @@
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="Y51" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z51" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA51" s="34" t="str">
         <f>$AA$20</f>
@@ -8983,7 +8983,7 @@
         <v>IND*</v>
       </c>
       <c r="Z52" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA52" s="22" t="s">
         <v>131</v>
@@ -9071,10 +9071,10 @@
         <v>I-DMD-PX4-E0</v>
       </c>
       <c r="Y53" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z53" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA53" s="22" t="s">
         <v>131</v>
@@ -9311,10 +9311,10 @@
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="Y57" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z57" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA57" s="34" t="str">
         <f>$AA$20</f>
@@ -9379,10 +9379,10 @@
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="Y58" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z58" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA58" s="34" t="str">
         <f>$AA$20</f>
@@ -9459,7 +9459,7 @@
         <v>IND*</v>
       </c>
       <c r="Z59" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA59" s="34" t="str">
         <f>$AA$20</f>
@@ -9539,10 +9539,10 @@
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="Y60" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z60" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA60" s="34" t="str">
         <f>$AA$20</f>
@@ -9619,7 +9619,7 @@
         <v>IND*</v>
       </c>
       <c r="Z61" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA61" s="22" t="s">
         <v>131</v>
@@ -9687,10 +9687,10 @@
         <v>I-DMD-CAF-E0</v>
       </c>
       <c r="Y62" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z62" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA62" s="22" t="s">
         <v>131</v>
@@ -9962,10 +9962,10 @@
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="Y68" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z68" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA68" s="34" t="str">
         <f>$AA$20</f>
@@ -10024,10 +10024,10 @@
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="Y69" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z69" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA69" s="34" t="str">
         <f>$AA$20</f>
@@ -10101,7 +10101,7 @@
         <v>IND*</v>
       </c>
       <c r="Z70" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA70" s="34" t="str">
         <f>$AA$20</f>
@@ -10169,10 +10169,10 @@
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="Y71" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z71" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA71" s="34" t="str">
         <f>$AA$20</f>
@@ -10237,7 +10237,7 @@
         <v>IND*</v>
       </c>
       <c r="Z72" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA72" s="22" t="s">
         <v>131</v>
@@ -10313,10 +10313,10 @@
         <v>I-DMD-RAP-E0</v>
       </c>
       <c r="Y73" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z73" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA73" s="22" t="s">
         <v>131</v>
@@ -10475,7 +10475,7 @@
         <v>132</v>
       </c>
       <c r="J77" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K77" s="14" t="s">
         <v>65</v>
@@ -10511,10 +10511,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y77" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z77" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA77" s="34" t="str">
         <f>$AA$20</f>
@@ -10554,7 +10554,7 @@
         <v>132</v>
       </c>
       <c r="J78" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K78" s="14" t="s">
         <v>67</v>
@@ -10582,10 +10582,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y78" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z78" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA78" s="34" t="str">
         <f>$AA$20</f>
@@ -10619,7 +10619,7 @@
         <v>132</v>
       </c>
       <c r="J79" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K79" s="14" t="s">
         <v>69</v>
@@ -10650,7 +10650,7 @@
         <v>IND*</v>
       </c>
       <c r="Z79" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA79" s="34" t="str">
         <f>$AA$20</f>
@@ -10690,7 +10690,7 @@
         <v>132</v>
       </c>
       <c r="J80" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K80" s="14" t="s">
         <v>70</v>
@@ -10718,10 +10718,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y80" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z80" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA80" s="34" t="str">
         <f>$AA$20</f>
@@ -10755,7 +10755,7 @@
         <v>132</v>
       </c>
       <c r="J81" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K81" s="14" t="s">
         <v>71</v>
@@ -10795,7 +10795,7 @@
         <v>IND*</v>
       </c>
       <c r="Z81" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA81" s="22" t="s">
         <v>131</v>
@@ -10834,7 +10834,7 @@
         <v>132</v>
       </c>
       <c r="J82" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K82" s="14" t="s">
         <v>72</v>
@@ -10862,10 +10862,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y82" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z82" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA82" s="22" t="s">
         <v>131</v>
@@ -10898,7 +10898,7 @@
         <v>132</v>
       </c>
       <c r="J83" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K83" s="14" t="s">
         <v>78</v>
@@ -10929,7 +10929,7 @@
         <v>IND*</v>
       </c>
       <c r="Z83" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA83" s="22" t="s">
         <v>131</v>
@@ -10968,7 +10968,7 @@
         <v>132</v>
       </c>
       <c r="J84" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K84" s="14" t="s">
         <v>81</v>
@@ -11008,10 +11008,10 @@
         <v>I-DMD-ONM-*</v>
       </c>
       <c r="Y84" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Z84" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA84" s="22" t="s">
         <v>131</v>
@@ -11044,7 +11044,7 @@
         <v>132</v>
       </c>
       <c r="J85" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K85" s="14" t="s">
         <v>87</v>
@@ -11076,7 +11076,7 @@
         <v>132</v>
       </c>
       <c r="J86" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K86" s="14" t="s">
         <v>88</v>
@@ -11108,7 +11108,7 @@
         <v>132</v>
       </c>
       <c r="J87" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K87" s="14" t="s">
         <v>109</v>
@@ -11155,7 +11155,7 @@
         <v>132</v>
       </c>
       <c r="J88" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K88" s="14" t="s">
         <v>110</v>
@@ -11202,7 +11202,7 @@
         <v>132</v>
       </c>
       <c r="J89" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K89" s="14" t="s">
         <v>80</v>
@@ -11249,10 +11249,10 @@
         <v>132</v>
       </c>
       <c r="J90" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K90" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L90" s="31">
         <v>0</v>
@@ -11358,10 +11358,10 @@
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="Y92" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z92" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA92" s="34" t="str">
         <f>$AA$20</f>
@@ -11429,10 +11429,10 @@
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="Y93" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z93" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA93" s="34" t="str">
         <f>$AA$20</f>
@@ -11497,7 +11497,7 @@
         <v>IND*</v>
       </c>
       <c r="Z94" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA94" s="34" t="str">
         <f>$AA$20</f>
@@ -11556,10 +11556,10 @@
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="Y95" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z95" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA95" s="34" t="str">
         <f>$AA$20</f>
@@ -11633,7 +11633,7 @@
         <v>IND*</v>
       </c>
       <c r="Z96" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA96" s="22" t="s">
         <v>131</v>
@@ -11709,10 +11709,10 @@
         <v>I-DMD-MAP-E0</v>
       </c>
       <c r="Y97" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z97" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA97" s="22" t="s">
         <v>131</v>
@@ -11974,10 +11974,10 @@
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="Y103" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z103" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA103" s="34" t="str">
         <f>$AA$20</f>
@@ -12036,10 +12036,10 @@
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="Y104" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z104" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA104" s="34" t="str">
         <f>$AA$20</f>
@@ -12113,7 +12113,7 @@
         <v>IND*</v>
       </c>
       <c r="Z105" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA105" s="34" t="str">
         <f>$AA$20</f>
@@ -12190,10 +12190,10 @@
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="Y106" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z106" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA106" s="34" t="str">
         <f>$AA$20</f>
@@ -12267,7 +12267,7 @@
         <v>IND*</v>
       </c>
       <c r="Z107" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA107" s="22" t="s">
         <v>131</v>
@@ -12343,10 +12343,10 @@
         <v>I-DMD-MAE-E0</v>
       </c>
       <c r="Y108" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z108" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA108" s="22" t="s">
         <v>131</v>
@@ -12523,10 +12523,10 @@
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="Y112" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z112" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA112" s="34" t="str">
         <f>$AA$20</f>
@@ -12585,10 +12585,10 @@
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="Y113" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z113" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA113" s="34" t="str">
         <f>$AA$20</f>
@@ -12662,7 +12662,7 @@
         <v>IND*</v>
       </c>
       <c r="Z114" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA114" s="34" t="str">
         <f>$AA$20</f>
@@ -12739,10 +12739,10 @@
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="Y115" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z115" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA115" s="34" t="str">
         <f>$AA$20</f>
@@ -12816,7 +12816,7 @@
         <v>IND*</v>
       </c>
       <c r="Z116" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA116" s="22" t="s">
         <v>131</v>
@@ -12892,10 +12892,10 @@
         <v>I-DMD-EOE-E0</v>
       </c>
       <c r="Y117" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z117" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA117" s="22" t="s">
         <v>131</v>
@@ -13072,10 +13072,10 @@
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="Y121" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z121" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA121" s="34" t="str">
         <f>$AA$20</f>
@@ -13134,10 +13134,10 @@
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="Y122" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z122" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA122" s="34" t="str">
         <f>$AA$20</f>
@@ -13211,7 +13211,7 @@
         <v>IND*</v>
       </c>
       <c r="Z123" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA123" s="34" t="str">
         <f>$AA$20</f>
@@ -13288,10 +13288,10 @@
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="Y124" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z124" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA124" s="34" t="str">
         <f>$AA$20</f>
@@ -13365,7 +13365,7 @@
         <v>IND*</v>
       </c>
       <c r="Z125" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA125" s="22" t="s">
         <v>131</v>
@@ -13441,10 +13441,10 @@
         <v>I-DMD-TEM-E0</v>
       </c>
       <c r="Y126" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z126" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA126" s="22" t="s">
         <v>131</v>
@@ -13621,10 +13621,10 @@
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="Y130" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z130" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA130" s="34" t="str">
         <f>$AA$20</f>
@@ -13683,10 +13683,10 @@
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="Y131" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z131" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA131" s="34" t="str">
         <f>$AA$20</f>
@@ -13751,7 +13751,7 @@
         <v>IND*</v>
       </c>
       <c r="Z132" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA132" s="34" t="str">
         <f>$AA$20</f>
@@ -13819,10 +13819,10 @@
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="Y133" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z133" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA133" s="34" t="str">
         <f>$AA$20</f>
@@ -13905,7 +13905,7 @@
         <v>IND*</v>
       </c>
       <c r="Z134" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA134" s="22" t="s">
         <v>131</v>
@@ -13972,10 +13972,10 @@
         <v>I-DMD-OMA-E0</v>
       </c>
       <c r="Y135" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z135" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA135" s="22" t="s">
         <v>131</v>
@@ -14199,10 +14199,10 @@
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="Y140" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z140" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA140" s="34" t="str">
         <f>$AA$20</f>
@@ -14261,10 +14261,10 @@
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="Y141" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z141" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA141" s="34" t="str">
         <f>$AA$20</f>
@@ -14338,7 +14338,7 @@
         <v>IND*</v>
       </c>
       <c r="Z142" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA142" s="34" t="str">
         <f>$AA$20</f>
@@ -14415,10 +14415,10 @@
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="Y143" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Z143" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA143" s="34" t="str">
         <f>$AA$20</f>
@@ -14492,7 +14492,7 @@
         <v>IND*</v>
       </c>
       <c r="Z144" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA144" s="22" t="s">
         <v>131</v>
@@ -14568,10 +14568,10 @@
         <v>I-DMD-CON-E0</v>
       </c>
       <c r="Y145" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z145" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AA145" s="22" t="s">
         <v>131</v>

</xml_diff>